<commit_message>
Database updated with One degree plan
</commit_message>
<xml_diff>
--- a/Docs/DatabaseSamples.xlsx
+++ b/Docs/DatabaseSamples.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s531367\Documents\44663\Team01Repo\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A8045398-F3D7-4F2D-B9F2-F0F1E0489B21}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8BE5667-9A97-4DBE-BACB-EDFD09EDB4D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="62">
   <si>
     <t>DegreeId</t>
   </si>
@@ -42,24 +42,6 @@
     <t xml:space="preserve">MS ACS +2 </t>
   </si>
   <si>
-    <t>ACS+DB</t>
-  </si>
-  <si>
-    <t>MS ACS +DB</t>
-  </si>
-  <si>
-    <t>ACS+NF</t>
-  </si>
-  <si>
-    <t>MS ACS+NF</t>
-  </si>
-  <si>
-    <t>ACS</t>
-  </si>
-  <si>
-    <t>MS ACS</t>
-  </si>
-  <si>
     <t>DegreeAbrrev(unique,max 6 characters)</t>
   </si>
   <si>
@@ -180,9 +162,6 @@
     <t>DegreePlanName(u,20)</t>
   </si>
   <si>
-    <t>S530473</t>
-  </si>
-  <si>
     <t>Summer Off</t>
   </si>
   <si>
@@ -210,9 +189,6 @@
     <t>Term Label</t>
   </si>
   <si>
-    <t>Fall 2017</t>
-  </si>
-  <si>
     <t>Spring 2018</t>
   </si>
   <si>
@@ -223,6 +199,24 @@
   </si>
   <si>
     <t>Spring 2019</t>
+  </si>
+  <si>
+    <t>S531367</t>
+  </si>
+  <si>
+    <t>Sai Sirisha</t>
+  </si>
+  <si>
+    <t>Devineni</t>
+  </si>
+  <si>
+    <t>s531367</t>
+  </si>
+  <si>
+    <t>Summer 2019</t>
+  </si>
+  <si>
+    <t>Fall 2019</t>
   </si>
 </sst>
 </file>
@@ -549,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A3" sqref="A3:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,10 +560,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -581,39 +575,6 @@
       </c>
       <c r="C2" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -638,13 +599,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -652,10 +613,10 @@
         <v>460</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -663,10 +624,10 @@
         <v>356</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -674,10 +635,10 @@
         <v>542</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -685,10 +646,10 @@
         <v>563</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -696,10 +657,10 @@
         <v>560</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -707,10 +668,10 @@
         <v>555</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -718,10 +679,10 @@
         <v>618</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -729,10 +690,10 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -740,10 +701,10 @@
         <v>664</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -751,10 +712,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -762,10 +723,10 @@
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -773,10 +734,10 @@
         <v>691</v>
       </c>
       <c r="B13" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -784,10 +745,10 @@
         <v>692</v>
       </c>
       <c r="B14" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -797,10 +758,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C49"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -812,13 +773,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -961,391 +922,6 @@
         <v>1</v>
       </c>
       <c r="C14">
-        <v>692</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15">
-        <v>2</v>
-      </c>
-      <c r="C15">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16">
-        <v>2</v>
-      </c>
-      <c r="C16">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <v>2</v>
-      </c>
-      <c r="C17">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18">
-        <v>2</v>
-      </c>
-      <c r="C18">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19">
-        <v>2</v>
-      </c>
-      <c r="C19">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20">
-        <v>2</v>
-      </c>
-      <c r="C20">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>20</v>
-      </c>
-      <c r="B21">
-        <v>2</v>
-      </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>21</v>
-      </c>
-      <c r="B22">
-        <v>2</v>
-      </c>
-      <c r="C22">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>22</v>
-      </c>
-      <c r="B23">
-        <v>2</v>
-      </c>
-      <c r="C23">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24">
-        <v>2</v>
-      </c>
-      <c r="C24">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>24</v>
-      </c>
-      <c r="B25">
-        <v>2</v>
-      </c>
-      <c r="C25">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26">
-        <v>2</v>
-      </c>
-      <c r="C26">
-        <v>692</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27">
-        <v>3</v>
-      </c>
-      <c r="C27">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28">
-        <v>3</v>
-      </c>
-      <c r="C28">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29">
-        <v>3</v>
-      </c>
-      <c r="C29">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30">
-        <v>3</v>
-      </c>
-      <c r="C30">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31">
-        <v>3</v>
-      </c>
-      <c r="C31">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="B32">
-        <v>3</v>
-      </c>
-      <c r="C32">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>32</v>
-      </c>
-      <c r="B33">
-        <v>3</v>
-      </c>
-      <c r="C33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>33</v>
-      </c>
-      <c r="B34">
-        <v>3</v>
-      </c>
-      <c r="C34">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>34</v>
-      </c>
-      <c r="B35">
-        <v>3</v>
-      </c>
-      <c r="C35">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>35</v>
-      </c>
-      <c r="B36">
-        <v>3</v>
-      </c>
-      <c r="C36">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>36</v>
-      </c>
-      <c r="B37">
-        <v>3</v>
-      </c>
-      <c r="C37">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>37</v>
-      </c>
-      <c r="B38">
-        <v>3</v>
-      </c>
-      <c r="C38">
-        <v>692</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>38</v>
-      </c>
-      <c r="B39">
-        <v>4</v>
-      </c>
-      <c r="C39">
-        <v>542</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>39</v>
-      </c>
-      <c r="B40">
-        <v>4</v>
-      </c>
-      <c r="C40">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>40</v>
-      </c>
-      <c r="B41">
-        <v>4</v>
-      </c>
-      <c r="C41">
-        <v>560</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>41</v>
-      </c>
-      <c r="B42">
-        <v>4</v>
-      </c>
-      <c r="C42">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>42</v>
-      </c>
-      <c r="B43">
-        <v>4</v>
-      </c>
-      <c r="C43">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>43</v>
-      </c>
-      <c r="B44">
-        <v>4</v>
-      </c>
-      <c r="C44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>44</v>
-      </c>
-      <c r="B45">
-        <v>4</v>
-      </c>
-      <c r="C45">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>45</v>
-      </c>
-      <c r="B46">
-        <v>4</v>
-      </c>
-      <c r="C46">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>46</v>
-      </c>
-      <c r="B47">
-        <v>4</v>
-      </c>
-      <c r="C47">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>47</v>
-      </c>
-      <c r="B48">
-        <v>4</v>
-      </c>
-      <c r="C48">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>48</v>
-      </c>
-      <c r="B49">
-        <v>4</v>
-      </c>
-      <c r="C49">
         <v>692</v>
       </c>
     </row>
@@ -1359,8 +935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1372,16 +948,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1758,7 +1334,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1770,19 +1346,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1793,13 +1369,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D2" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="E2" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1810,13 +1386,13 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="E3" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1829,23 +1405,23 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" t="s">
         <v>47</v>
       </c>
-      <c r="B1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C1" t="s">
-        <v>54</v>
-      </c>
       <c r="D1" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="E1">
         <v>919</v>
@@ -1853,7 +1429,19 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>530473</v>
+        <v>531367</v>
+      </c>
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2">
+        <v>562438</v>
       </c>
     </row>
   </sheetData>
@@ -1863,26 +1451,32 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="19" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="D1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1890,13 +1484,13 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>530473</v>
+        <v>531367</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1904,13 +1498,13 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>530473</v>
+        <v>531367</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1918,13 +1512,13 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>530473</v>
+        <v>531367</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1932,13 +1526,13 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>530473</v>
+        <v>531367</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1946,13 +1540,27 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>530473</v>
+        <v>531367</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>63</v>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>531367</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
change in xcel sheet
</commit_message>
<xml_diff>
--- a/Docs/DatabaseSamples.xlsx
+++ b/Docs/DatabaseSamples.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s531367\Documents\44663\Team01Repo\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S533985\Documents\44663\Team01Repo\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8BE5667-9A97-4DBE-BACB-EDFD09EDB4D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="65">
   <si>
     <t>DegreeId</t>
   </si>
@@ -217,12 +216,21 @@
   </si>
   <si>
     <t>Fall 2019</t>
+  </si>
+  <si>
+    <t>Dristi</t>
+  </si>
+  <si>
+    <t>Marasini</t>
+  </si>
+  <si>
+    <t>s533985</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -542,7 +550,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -584,7 +592,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
@@ -757,10 +765,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -932,7 +940,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView topLeftCell="A8" workbookViewId="0">
@@ -1330,7 +1338,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1401,11 +1409,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1444,17 +1452,34 @@
         <v>562438</v>
       </c>
     </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>533985</v>
+      </c>
+      <c r="B3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3">
+        <v>569178</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:D7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1563,6 +1588,76 @@
         <v>61</v>
       </c>
     </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>533985</v>
+      </c>
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>533985</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>533985</v>
+      </c>
+      <c r="C10">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>533985</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>533985</v>
+      </c>
+      <c r="C12">
+        <v>11</v>
+      </c>
+      <c r="D12" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated the Excel sheet with the new a student and new student term.
</commit_message>
<xml_diff>
--- a/Docs/DatabaseSamples.xlsx
+++ b/Docs/DatabaseSamples.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S533985\Documents\44663\Team01Repo\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\44663\Team01Repo\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="68">
   <si>
     <t>DegreeId</t>
   </si>
@@ -225,6 +225,15 @@
   </si>
   <si>
     <t>s533985</t>
+  </si>
+  <si>
+    <t>Aawaj</t>
+  </si>
+  <si>
+    <t>Joshi</t>
+  </si>
+  <si>
+    <t>s521315</t>
   </si>
 </sst>
 </file>
@@ -1410,10 +1419,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1469,6 +1478,23 @@
         <v>569178</v>
       </c>
     </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>521315</v>
+      </c>
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4">
+        <v>480684</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1476,10 +1502,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1658,6 +1684,76 @@
         <v>55</v>
       </c>
     </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>521315</v>
+      </c>
+      <c r="C13">
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>521315</v>
+      </c>
+      <c r="C14">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>521315</v>
+      </c>
+      <c r="C15">
+        <v>14</v>
+      </c>
+      <c r="D15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>521315</v>
+      </c>
+      <c r="C16">
+        <v>15</v>
+      </c>
+      <c r="D16" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>521315</v>
+      </c>
+      <c r="C17">
+        <v>16</v>
+      </c>
+      <c r="D17" t="s">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated the DegreePlan sheet
</commit_message>
<xml_diff>
--- a/Docs/DatabaseSamples.xlsx
+++ b/Docs/DatabaseSamples.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\masters\C#.net\Team01Repo\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\44663\Team01Repo\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="73">
   <si>
     <t>DegreeId</t>
   </si>
@@ -243,6 +243,12 @@
   </si>
   <si>
     <t>s533900</t>
+  </si>
+  <si>
+    <t>S521315</t>
+  </si>
+  <si>
+    <t>S533985</t>
   </si>
 </sst>
 </file>
@@ -1357,10 +1363,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1418,6 +1424,74 @@
         <v>43</v>
       </c>
       <c r="E3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1530,7 +1604,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated a few sheets.
</commit_message>
<xml_diff>
--- a/Docs/DatabaseSamples.xlsx
+++ b/Docs/DatabaseSamples.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\masters\C#.net\Team01Repo\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\44663\Team01Repo\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" firstSheet="2" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="73">
   <si>
     <t>DegreeId</t>
   </si>
@@ -272,7 +272,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -291,6 +291,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -304,13 +316,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -594,7 +608,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1046,10 +1060,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D79"/>
+  <dimension ref="A1:D105"/>
   <sheetViews>
-    <sheetView topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
+      <selection activeCell="B109" sqref="B109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2165,6 +2179,370 @@
         <v>555</v>
       </c>
     </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="6">
+        <v>79</v>
+      </c>
+      <c r="B80" s="6">
+        <v>14</v>
+      </c>
+      <c r="C80" s="6">
+        <v>1</v>
+      </c>
+      <c r="D80" s="6">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="6">
+        <v>80</v>
+      </c>
+      <c r="B81" s="6">
+        <v>14</v>
+      </c>
+      <c r="C81" s="6">
+        <v>1</v>
+      </c>
+      <c r="D81" s="6">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="6">
+        <v>81</v>
+      </c>
+      <c r="B82" s="6">
+        <v>14</v>
+      </c>
+      <c r="C82" s="6">
+        <v>1</v>
+      </c>
+      <c r="D82" s="6">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="6">
+        <v>82</v>
+      </c>
+      <c r="B83" s="6">
+        <v>14</v>
+      </c>
+      <c r="C83" s="6">
+        <v>1</v>
+      </c>
+      <c r="D83" s="6">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="6">
+        <v>83</v>
+      </c>
+      <c r="B84" s="6">
+        <v>14</v>
+      </c>
+      <c r="C84" s="6">
+        <v>2</v>
+      </c>
+      <c r="D84" s="6">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="6">
+        <v>84</v>
+      </c>
+      <c r="B85" s="6">
+        <v>14</v>
+      </c>
+      <c r="C85" s="6">
+        <v>2</v>
+      </c>
+      <c r="D85" s="6">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="6">
+        <v>85</v>
+      </c>
+      <c r="B86" s="6">
+        <v>14</v>
+      </c>
+      <c r="C86" s="6">
+        <v>2</v>
+      </c>
+      <c r="D86" s="6">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="6">
+        <v>86</v>
+      </c>
+      <c r="B87" s="6">
+        <v>14</v>
+      </c>
+      <c r="C87" s="6">
+        <v>4</v>
+      </c>
+      <c r="D87" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="6">
+        <v>87</v>
+      </c>
+      <c r="B88" s="6">
+        <v>14</v>
+      </c>
+      <c r="C88" s="6">
+        <v>4</v>
+      </c>
+      <c r="D88" s="6">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="6">
+        <v>88</v>
+      </c>
+      <c r="B89" s="6">
+        <v>14</v>
+      </c>
+      <c r="C89" s="6">
+        <v>4</v>
+      </c>
+      <c r="D89" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="6">
+        <v>89</v>
+      </c>
+      <c r="B90" s="6">
+        <v>14</v>
+      </c>
+      <c r="C90" s="6">
+        <v>5</v>
+      </c>
+      <c r="D90" s="6">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="6">
+        <v>90</v>
+      </c>
+      <c r="B91" s="6">
+        <v>14</v>
+      </c>
+      <c r="C91" s="6">
+        <v>5</v>
+      </c>
+      <c r="D91" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="6">
+        <v>91</v>
+      </c>
+      <c r="B92" s="6">
+        <v>14</v>
+      </c>
+      <c r="C92" s="6">
+        <v>5</v>
+      </c>
+      <c r="D92" s="6">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="6">
+        <v>92</v>
+      </c>
+      <c r="B93" s="6">
+        <v>15</v>
+      </c>
+      <c r="C93" s="6">
+        <v>1</v>
+      </c>
+      <c r="D93" s="6">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="6">
+        <v>93</v>
+      </c>
+      <c r="B94" s="6">
+        <v>15</v>
+      </c>
+      <c r="C94" s="6">
+        <v>1</v>
+      </c>
+      <c r="D94" s="6">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="6">
+        <v>94</v>
+      </c>
+      <c r="B95" s="6">
+        <v>15</v>
+      </c>
+      <c r="C95" s="6">
+        <v>1</v>
+      </c>
+      <c r="D95" s="6">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="6">
+        <v>95</v>
+      </c>
+      <c r="B96" s="6">
+        <v>15</v>
+      </c>
+      <c r="C96" s="6">
+        <v>1</v>
+      </c>
+      <c r="D96" s="6">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="6">
+        <v>96</v>
+      </c>
+      <c r="B97" s="6">
+        <v>15</v>
+      </c>
+      <c r="C97" s="6">
+        <v>2</v>
+      </c>
+      <c r="D97" s="6">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="6">
+        <v>97</v>
+      </c>
+      <c r="B98" s="6">
+        <v>15</v>
+      </c>
+      <c r="C98" s="6">
+        <v>2</v>
+      </c>
+      <c r="D98" s="6">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="6">
+        <v>98</v>
+      </c>
+      <c r="B99" s="6">
+        <v>15</v>
+      </c>
+      <c r="C99" s="6">
+        <v>2</v>
+      </c>
+      <c r="D99" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="6">
+        <v>99</v>
+      </c>
+      <c r="B100" s="6">
+        <v>15</v>
+      </c>
+      <c r="C100" s="6">
+        <v>3</v>
+      </c>
+      <c r="D100" s="6">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="6">
+        <v>100</v>
+      </c>
+      <c r="B101" s="6">
+        <v>15</v>
+      </c>
+      <c r="C101" s="6">
+        <v>3</v>
+      </c>
+      <c r="D101" s="6">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="6">
+        <v>101</v>
+      </c>
+      <c r="B102" s="6">
+        <v>15</v>
+      </c>
+      <c r="C102" s="6">
+        <v>3</v>
+      </c>
+      <c r="D102" s="6">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="6">
+        <v>102</v>
+      </c>
+      <c r="B103" s="6">
+        <v>15</v>
+      </c>
+      <c r="C103" s="6">
+        <v>4</v>
+      </c>
+      <c r="D103" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="6">
+        <v>103</v>
+      </c>
+      <c r="B104" s="6">
+        <v>15</v>
+      </c>
+      <c r="C104" s="6">
+        <v>4</v>
+      </c>
+      <c r="D104" s="6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" s="6">
+        <v>104</v>
+      </c>
+      <c r="B105" s="6">
+        <v>15</v>
+      </c>
+      <c r="C105" s="6">
+        <v>4</v>
+      </c>
+      <c r="D105" s="6">
+        <v>692</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -2173,10 +2551,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2307,6 +2685,42 @@
         <v>45</v>
       </c>
     </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>14</v>
+      </c>
+      <c r="B8" s="7">
+        <v>1</v>
+      </c>
+      <c r="C8" s="7">
+        <v>521315</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>15</v>
+      </c>
+      <c r="B9" s="7">
+        <v>1</v>
+      </c>
+      <c r="C9" s="7">
+        <v>521315</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F9" s="7"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2317,7 +2731,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E4" sqref="A4:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2374,19 +2788,19 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="6">
         <v>521315</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="6">
         <v>480684</v>
       </c>
     </row>
@@ -2416,8 +2830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2611,72 +3025,72 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14">
+      <c r="A14" s="6">
         <v>13</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="6">
         <v>521315</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="6">
         <v>12</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="6" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
+      <c r="A15" s="6">
         <v>14</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="6">
         <v>521315</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="6">
         <v>13</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="6" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="6">
         <v>15</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="6">
         <v>521315</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="6">
         <v>14</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="6" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
+      <c r="A17" s="6">
         <v>16</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="6">
         <v>521315</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="6">
         <v>15</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="6" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="A18" s="6">
         <v>17</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="6">
         <v>521315</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="6">
         <v>16</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="6" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Models/Degree.cs Models/Requirement.cs and made corrections to Models/DegreePlan.cs
</commit_message>
<xml_diff>
--- a/Docs/DatabaseSamples.xlsx
+++ b/Docs/DatabaseSamples.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\44663\Team01Repo\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s531367\Documents\44663\Team01Repo\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92162C3-5D37-42E1-B86D-ADE807ED5236}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
@@ -30,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="73">
-  <si>
-    <t>DegreeId</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="69">
   <si>
     <t>ACS+2</t>
   </si>
@@ -128,36 +126,18 @@
     <t>GDP2</t>
   </si>
   <si>
-    <t>DegreeRequirementId</t>
-  </si>
-  <si>
-    <t>RequirementId</t>
-  </si>
-  <si>
     <t>StudentID</t>
   </si>
   <si>
     <t>DegreePlanID</t>
   </si>
   <si>
-    <t>TermId</t>
-  </si>
-  <si>
-    <t>DegreePlanTermRequirementId</t>
-  </si>
-  <si>
-    <t>DegreePlanId</t>
-  </si>
-  <si>
     <t>DegreeID</t>
   </si>
   <si>
     <t>DegreePlanAbbrev(u,8)</t>
   </si>
   <si>
-    <t>StudentId</t>
-  </si>
-  <si>
     <t>DegreePlanName(u,20)</t>
   </si>
   <si>
@@ -179,15 +159,9 @@
     <t>Snumber</t>
   </si>
   <si>
-    <t>StudentTermId</t>
-  </si>
-  <si>
     <t>Term</t>
   </si>
   <si>
-    <t>Term Label</t>
-  </si>
-  <si>
     <t>Spring 2018</t>
   </si>
   <si>
@@ -249,12 +223,27 @@
   </si>
   <si>
     <t>Fall2019</t>
+  </si>
+  <si>
+    <t>DegreeRequirementID</t>
+  </si>
+  <si>
+    <t>DegreePlanTermRequirementID</t>
+  </si>
+  <si>
+    <t>TermID</t>
+  </si>
+  <si>
+    <t>StudentTermID</t>
+  </si>
+  <si>
+    <t>TermLabel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -604,12 +593,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -619,13 +606,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -633,10 +620,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -646,28 +633,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="22.42578125" customWidth="1"/>
     <col min="2" max="2" width="34.85546875" customWidth="1"/>
     <col min="3" max="3" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
         <v>19</v>
-      </c>
-      <c r="C1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -675,10 +661,10 @@
         <v>460</v>
       </c>
       <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -686,10 +672,10 @@
         <v>356</v>
       </c>
       <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -697,10 +683,10 @@
         <v>542</v>
       </c>
       <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
         <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -708,10 +694,10 @@
         <v>563</v>
       </c>
       <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
         <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -719,10 +705,10 @@
         <v>560</v>
       </c>
       <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
         <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -730,10 +716,10 @@
         <v>555</v>
       </c>
       <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
         <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -741,10 +727,10 @@
         <v>618</v>
       </c>
       <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
         <v>17</v>
-      </c>
-      <c r="C8" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -752,10 +738,10 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
         <v>22</v>
-      </c>
-      <c r="C9" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -763,10 +749,10 @@
         <v>664</v>
       </c>
       <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
         <v>24</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -774,10 +760,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -785,10 +771,10 @@
         <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -796,10 +782,10 @@
         <v>691</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -807,10 +793,10 @@
         <v>692</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -819,11 +805,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -835,13 +821,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="C1" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1059,11 +1045,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" workbookViewId="0">
-      <selection activeCell="B109" sqref="B109"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1075,16 +1061,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="D1" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2550,12 +2536,10 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2566,19 +2550,19 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E1" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -2592,10 +2576,10 @@
         <v>531367</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E2" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -2609,10 +2593,10 @@
         <v>531367</v>
       </c>
       <c r="D3" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E3" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -2626,10 +2610,10 @@
         <v>533900</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F4" s="3"/>
     </row>
@@ -2644,10 +2628,10 @@
         <v>533900</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F5" s="3"/>
     </row>
@@ -2662,10 +2646,10 @@
         <v>533985</v>
       </c>
       <c r="D6" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E6" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -2679,10 +2663,10 @@
         <v>533985</v>
       </c>
       <c r="D7" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -2696,10 +2680,10 @@
         <v>521315</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F8" s="7"/>
     </row>
@@ -2714,10 +2698,10 @@
         <v>521315</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F9" s="7"/>
     </row>
@@ -2727,27 +2711,25 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="A4:E4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
         <v>41</v>
-      </c>
-      <c r="B1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" t="s">
-        <v>48</v>
       </c>
       <c r="E1">
         <v>919</v>
@@ -2758,13 +2740,13 @@
         <v>531367</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E2">
         <v>562438</v>
@@ -2775,13 +2757,13 @@
         <v>533985</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C3" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="E3">
         <v>569178</v>
@@ -2792,13 +2774,13 @@
         <v>521315</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="E4" s="6">
         <v>480684</v>
@@ -2809,13 +2791,13 @@
         <v>533900</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="E5" s="3">
         <v>568896</v>
@@ -2827,11 +2809,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2844,16 +2826,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>67</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C1" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D1" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -2867,7 +2849,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -2881,7 +2863,7 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -2895,7 +2877,7 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2909,7 +2891,7 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2923,7 +2905,7 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -2937,7 +2919,7 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -2951,7 +2933,7 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2965,7 +2947,7 @@
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -2979,7 +2961,7 @@
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2993,7 +2975,7 @@
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -3007,7 +2989,7 @@
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -3021,7 +3003,7 @@
         <v>6</v>
       </c>
       <c r="D13" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -3035,7 +3017,7 @@
         <v>12</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -3049,7 +3031,7 @@
         <v>13</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -3063,7 +3045,7 @@
         <v>14</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3077,7 +3059,7 @@
         <v>15</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -3091,7 +3073,7 @@
         <v>16</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -3105,7 +3087,7 @@
         <v>17</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -3119,7 +3101,7 @@
         <v>18</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -3133,7 +3115,7 @@
         <v>19</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -3147,7 +3129,7 @@
         <v>20</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -3161,7 +3143,7 @@
         <v>21</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
formula added in the document
</commit_message>
<xml_diff>
--- a/Docs/DatabaseSamples.xlsx
+++ b/Docs/DatabaseSamples.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s531367\Documents\44663\Team01Repo\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\S533985\Documents\44663\Team01Repo\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92162C3-5D37-42E1-B86D-ADE807ED5236}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="6945" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Degree" sheetId="1" r:id="rId1"/>
@@ -31,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="70">
   <si>
     <t>ACS+2</t>
   </si>
@@ -238,13 +237,16 @@
   </si>
   <si>
     <t>TermLabel</t>
+  </si>
+  <si>
+    <t>string</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -256,6 +258,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -305,7 +314,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -314,6 +323,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -593,18 +606,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.7109375" customWidth="1"/>
     <col min="2" max="2" width="36.7109375" customWidth="1"/>
+    <col min="3" max="3" width="42.28515625" customWidth="1"/>
+    <col min="4" max="4" width="52.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
@@ -615,7 +632,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -624,6 +641,10 @@
       </c>
       <c r="C2" t="s">
         <v>1</v>
+      </c>
+      <c r="D2" s="8" t="str">
+        <f>C2&amp;$A$1&amp;"="&amp;A2&amp;","</f>
+        <v>MS ACS +2 DegreeID=1,</v>
       </c>
     </row>
   </sheetData>
@@ -633,7 +654,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -805,7 +826,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1045,11 +1066,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D105"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E105"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1057,9 +1078,10 @@
     <col min="1" max="1" width="34.5703125" customWidth="1"/>
     <col min="2" max="2" width="30.7109375" customWidth="1"/>
     <col min="4" max="4" width="25.85546875" customWidth="1"/>
+    <col min="5" max="5" width="85.7109375" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>65</v>
       </c>
@@ -1072,8 +1094,11 @@
       <c r="D1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1086,8 +1111,12 @@
       <c r="D2">
         <v>460</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="9" t="str">
+        <f>"new DegreePlanTermRequirement{"&amp;$A$1&amp;"="&amp;A2&amp;$B$1&amp;"="&amp;B2&amp;$C$1&amp;"="&amp;C2&amp;$D$1&amp;"="&amp;D2</f>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=1DegreePlanID=10TermID=1RequirementID=460</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1100,8 +1129,12 @@
       <c r="D3">
         <v>356</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="9" t="str">
+        <f>"new DegreePlanTermRequirement{"&amp;$A$1&amp;"="&amp;A3&amp;$B$1&amp;"="&amp;B3&amp;$C$1&amp;"="&amp;C3&amp;$D$1&amp;"="&amp;D3</f>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=2DegreePlanID=10TermID=1RequirementID=356</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1114,8 +1147,12 @@
       <c r="D4">
         <v>542</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="9" t="str">
+        <f t="shared" ref="E3:E66" si="0">"new DegreePlanTermRequirement{"&amp;$A$1&amp;"="&amp;A4&amp;$B$1&amp;"="&amp;B4&amp;$C$1&amp;"="&amp;C4&amp;$D$1&amp;"="&amp;D4</f>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=3DegreePlanID=10TermID=1RequirementID=542</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1128,8 +1165,12 @@
       <c r="D5">
         <v>563</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=4DegreePlanID=10TermID=1RequirementID=563</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1142,8 +1183,12 @@
       <c r="D6">
         <v>560</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=5DegreePlanID=10TermID=2RequirementID=560</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1156,8 +1201,12 @@
       <c r="D7">
         <v>555</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=6DegreePlanID=10TermID=2RequirementID=555</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1170,8 +1219,12 @@
       <c r="D8">
         <v>618</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=7DegreePlanID=10TermID=2RequirementID=618</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1184,8 +1237,12 @@
       <c r="D9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=8DegreePlanID=10TermID=3RequirementID=1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1198,8 +1255,12 @@
       <c r="D10">
         <v>664</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=9DegreePlanID=10TermID=3RequirementID=664</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1212,8 +1273,12 @@
       <c r="D11">
         <v>691</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=10DegreePlanID=10TermID=3RequirementID=691</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1226,8 +1291,12 @@
       <c r="D12">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=11DegreePlanID=10TermID=4RequirementID=10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1240,8 +1309,12 @@
       <c r="D13">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=12DegreePlanID=10TermID=4RequirementID=20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1254,8 +1327,12 @@
       <c r="D14">
         <v>692</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=13DegreePlanID=10TermID=4RequirementID=692</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1268,8 +1345,12 @@
       <c r="D15">
         <v>460</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=14DegreePlanID=11TermID=1RequirementID=460</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1282,8 +1363,12 @@
       <c r="D16">
         <v>356</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=15DegreePlanID=11TermID=1RequirementID=356</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1296,8 +1381,12 @@
       <c r="D17">
         <v>542</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=16DegreePlanID=11TermID=1RequirementID=542</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1310,8 +1399,12 @@
       <c r="D18">
         <v>563</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=17DegreePlanID=11TermID=1RequirementID=563</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1324,8 +1417,12 @@
       <c r="D19">
         <v>560</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=18DegreePlanID=11TermID=2RequirementID=560</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1338,8 +1435,12 @@
       <c r="D20">
         <v>555</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=19DegreePlanID=11TermID=2RequirementID=555</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1352,8 +1453,12 @@
       <c r="D21">
         <v>618</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=20DegreePlanID=11TermID=2RequirementID=618</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1366,8 +1471,12 @@
       <c r="D22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=21DegreePlanID=11TermID=4RequirementID=1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1380,8 +1489,12 @@
       <c r="D23">
         <v>664</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=22DegreePlanID=11TermID=4RequirementID=664</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1394,8 +1507,12 @@
       <c r="D24">
         <v>691</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=23DegreePlanID=11TermID=4RequirementID=691</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1408,8 +1525,12 @@
       <c r="D25">
         <v>10</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=24DegreePlanID=11TermID=5RequirementID=10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1422,8 +1543,12 @@
       <c r="D26">
         <v>20</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=25DegreePlanID=11TermID=5RequirementID=20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1436,8 +1561,12 @@
       <c r="D27">
         <v>692</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=26DegreePlanID=11TermID=5RequirementID=692</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -1450,8 +1579,12 @@
       <c r="D28" s="3">
         <v>460</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=27DegreePlanID=30TermID=18RequirementID=460</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -1464,8 +1597,12 @@
       <c r="D29" s="3">
         <v>356</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=28DegreePlanID=30TermID=18RequirementID=356</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -1478,8 +1615,12 @@
       <c r="D30" s="3">
         <v>542</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=29DegreePlanID=30TermID=18RequirementID=542</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -1492,8 +1633,12 @@
       <c r="D31" s="3">
         <v>563</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=30DegreePlanID=30TermID=18RequirementID=563</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -1506,8 +1651,12 @@
       <c r="D32" s="3">
         <v>560</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=31DegreePlanID=30TermID=19RequirementID=560</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -1520,8 +1669,12 @@
       <c r="D33" s="3">
         <v>555</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=32DegreePlanID=30TermID=19RequirementID=555</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -1534,8 +1687,12 @@
       <c r="D34" s="3">
         <v>618</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=33DegreePlanID=30TermID=19RequirementID=618</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -1548,8 +1705,12 @@
       <c r="D35" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=34DegreePlanID=30TermID=21RequirementID=1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -1562,8 +1723,12 @@
       <c r="D36" s="3">
         <v>664</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=35DegreePlanID=30TermID=21RequirementID=664</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -1576,8 +1741,12 @@
       <c r="D37" s="3">
         <v>691</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=36DegreePlanID=30TermID=21RequirementID=691</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -1590,8 +1759,12 @@
       <c r="D38" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=37DegreePlanID=30TermID=21RequirementID=10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -1604,8 +1777,12 @@
       <c r="D39" s="3">
         <v>20</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=38DegreePlanID=30TermID=22RequirementID=20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -1618,8 +1795,12 @@
       <c r="D40" s="3">
         <v>692</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=39DegreePlanID=30TermID=22RequirementID=692</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -1632,8 +1813,12 @@
       <c r="D41" s="3">
         <v>460</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=40DegreePlanID=31TermID=18RequirementID=460</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>41</v>
       </c>
@@ -1646,8 +1831,12 @@
       <c r="D42" s="3">
         <v>356</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=41DegreePlanID=31TermID=18RequirementID=356</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>42</v>
       </c>
@@ -1660,8 +1849,12 @@
       <c r="D43" s="3">
         <v>542</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=42DegreePlanID=31TermID=18RequirementID=542</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>43</v>
       </c>
@@ -1674,8 +1867,12 @@
       <c r="D44" s="3">
         <v>563</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=43DegreePlanID=31TermID=18RequirementID=563</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>44</v>
       </c>
@@ -1688,8 +1885,12 @@
       <c r="D45" s="3">
         <v>560</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=44DegreePlanID=31TermID=19RequirementID=560</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>45</v>
       </c>
@@ -1702,8 +1903,12 @@
       <c r="D46" s="3">
         <v>555</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=45DegreePlanID=31TermID=19RequirementID=555</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>46</v>
       </c>
@@ -1716,8 +1921,12 @@
       <c r="D47" s="3">
         <v>618</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E47" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=46DegreePlanID=31TermID=19RequirementID=618</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>47</v>
       </c>
@@ -1730,8 +1939,12 @@
       <c r="D48" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=47DegreePlanID=31TermID=20RequirementID=1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>48</v>
       </c>
@@ -1744,8 +1957,12 @@
       <c r="D49" s="3">
         <v>664</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=48DegreePlanID=31TermID=21RequirementID=664</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>49</v>
       </c>
@@ -1758,8 +1975,12 @@
       <c r="D50" s="3">
         <v>691</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=49DegreePlanID=31TermID=21RequirementID=691</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>50</v>
       </c>
@@ -1772,8 +1993,12 @@
       <c r="D51" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=50DegreePlanID=31TermID=21RequirementID=10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>51</v>
       </c>
@@ -1786,8 +2011,12 @@
       <c r="D52" s="3">
         <v>20</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=51DegreePlanID=31TermID=22RequirementID=20</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>52</v>
       </c>
@@ -1800,8 +2029,12 @@
       <c r="D53" s="3">
         <v>692</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E53" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=52DegreePlanID=31TermID=22RequirementID=692</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>53</v>
       </c>
@@ -1814,8 +2047,12 @@
       <c r="D54" s="4">
         <v>542</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E54" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=53DegreePlanID=12TermID=1RequirementID=542</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>54</v>
       </c>
@@ -1828,8 +2065,12 @@
       <c r="D55" s="4">
         <v>460</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E55" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=54DegreePlanID=12TermID=1RequirementID=460</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>55</v>
       </c>
@@ -1842,8 +2083,12 @@
       <c r="D56" s="4">
         <v>356</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E56" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=55DegreePlanID=12TermID=1RequirementID=356</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>56</v>
       </c>
@@ -1856,8 +2101,12 @@
       <c r="D57" s="4">
         <v>664</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E57" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=56DegreePlanID=12TermID=3RequirementID=664</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
         <v>57</v>
       </c>
@@ -1870,8 +2119,12 @@
       <c r="D58" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E58" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=57DegreePlanID=12TermID=3RequirementID=1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
         <v>58</v>
       </c>
@@ -1884,8 +2137,12 @@
       <c r="D59" s="4">
         <v>560</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E59" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=58DegreePlanID=12TermID=3RequirementID=560</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
         <v>59</v>
       </c>
@@ -1898,8 +2155,12 @@
       <c r="D60" s="4">
         <v>691</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E60" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=59DegreePlanID=12TermID=2RequirementID=691</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
         <v>60</v>
       </c>
@@ -1912,8 +2173,12 @@
       <c r="D61" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E61" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=60DegreePlanID=12TermID=2RequirementID=10</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>61</v>
       </c>
@@ -1926,8 +2191,12 @@
       <c r="D62" s="4">
         <v>692</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E62" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=61DegreePlanID=12TermID=4RequirementID=692</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <v>62</v>
       </c>
@@ -1940,8 +2209,12 @@
       <c r="D63" s="4">
         <v>555</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E63" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=62DegreePlanID=12TermID=4RequirementID=555</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <v>63</v>
       </c>
@@ -1954,8 +2227,12 @@
       <c r="D64" s="4">
         <v>563</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E64" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=63DegreePlanID=12TermID=6RequirementID=563</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>64</v>
       </c>
@@ -1968,8 +2245,12 @@
       <c r="D65" s="4">
         <v>20</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E65" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=64DegreePlanID=12TermID=6RequirementID=20</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
         <v>65</v>
       </c>
@@ -1982,8 +2263,12 @@
       <c r="D66" s="4">
         <v>618</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E66" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=65DegreePlanID=12TermID=6RequirementID=618</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
         <v>66</v>
       </c>
@@ -1996,8 +2281,12 @@
       <c r="D67" s="4">
         <v>356</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E67" s="9" t="str">
+        <f t="shared" ref="E67:E105" si="1">"new DegreePlanTermRequirement{"&amp;$A$1&amp;"="&amp;A67&amp;$B$1&amp;"="&amp;B67&amp;$C$1&amp;"="&amp;C67&amp;$D$1&amp;"="&amp;D67</f>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=66DegreePlanID=13TermID=1RequirementID=356</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
         <v>67</v>
       </c>
@@ -2010,8 +2299,12 @@
       <c r="D68" s="4">
         <v>460</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E68" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=67DegreePlanID=13TermID=1RequirementID=460</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
         <v>68</v>
       </c>
@@ -2024,8 +2317,12 @@
       <c r="D69" s="4">
         <v>542</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E69" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=68DegreePlanID=13TermID=1RequirementID=542</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
         <v>69</v>
       </c>
@@ -2038,8 +2335,12 @@
       <c r="D70" s="4">
         <v>563</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E70" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=69DegreePlanID=13TermID=1RequirementID=563</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
         <v>70</v>
       </c>
@@ -2052,8 +2353,12 @@
       <c r="D71" s="4">
         <v>560</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E71" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=70DegreePlanID=13TermID=3RequirementID=560</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
         <v>71</v>
       </c>
@@ -2066,8 +2371,12 @@
       <c r="D72" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E72" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=71DegreePlanID=13TermID=3RequirementID=1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A73" s="4">
         <v>72</v>
       </c>
@@ -2080,8 +2389,12 @@
       <c r="D73" s="4">
         <v>664</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E73" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=72DegreePlanID=13TermID=3RequirementID=664</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
         <v>73</v>
       </c>
@@ -2094,8 +2407,12 @@
       <c r="D74" s="4">
         <v>10</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E74" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=73DegreePlanID=13TermID=3RequirementID=10</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A75" s="4">
         <v>74</v>
       </c>
@@ -2108,8 +2425,12 @@
       <c r="D75" s="4">
         <v>20</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E75" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=74DegreePlanID=13TermID=4RequirementID=20</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A76" s="4">
         <v>75</v>
       </c>
@@ -2122,8 +2443,12 @@
       <c r="D76" s="4">
         <v>691</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E76" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=75DegreePlanID=13TermID=4RequirementID=691</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A77" s="4">
         <v>76</v>
       </c>
@@ -2136,8 +2461,12 @@
       <c r="D77" s="4">
         <v>618</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E77" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=76DegreePlanID=13TermID=4RequirementID=618</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A78" s="4">
         <v>77</v>
       </c>
@@ -2150,8 +2479,12 @@
       <c r="D78" s="4">
         <v>692</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E78" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=77DegreePlanID=13TermID=6RequirementID=692</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A79" s="4">
         <v>78</v>
       </c>
@@ -2164,8 +2497,12 @@
       <c r="D79" s="4">
         <v>555</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E79" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=78DegreePlanID=13TermID=6RequirementID=555</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A80" s="6">
         <v>79</v>
       </c>
@@ -2178,8 +2515,12 @@
       <c r="D80" s="6">
         <v>460</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E80" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=79DegreePlanID=14TermID=1RequirementID=460</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A81" s="6">
         <v>80</v>
       </c>
@@ -2192,8 +2533,12 @@
       <c r="D81" s="6">
         <v>356</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E81" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=80DegreePlanID=14TermID=1RequirementID=356</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A82" s="6">
         <v>81</v>
       </c>
@@ -2206,8 +2551,12 @@
       <c r="D82" s="6">
         <v>542</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E82" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=81DegreePlanID=14TermID=1RequirementID=542</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A83" s="6">
         <v>82</v>
       </c>
@@ -2220,8 +2569,12 @@
       <c r="D83" s="6">
         <v>563</v>
       </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E83" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=82DegreePlanID=14TermID=1RequirementID=563</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A84" s="6">
         <v>83</v>
       </c>
@@ -2234,8 +2587,12 @@
       <c r="D84" s="6">
         <v>560</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E84" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=83DegreePlanID=14TermID=2RequirementID=560</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A85" s="6">
         <v>84</v>
       </c>
@@ -2248,8 +2605,12 @@
       <c r="D85" s="6">
         <v>555</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E85" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=84DegreePlanID=14TermID=2RequirementID=555</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A86" s="6">
         <v>85</v>
       </c>
@@ -2262,8 +2623,12 @@
       <c r="D86" s="6">
         <v>664</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E86" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=85DegreePlanID=14TermID=2RequirementID=664</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A87" s="6">
         <v>86</v>
       </c>
@@ -2276,8 +2641,12 @@
       <c r="D87" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E87" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=86DegreePlanID=14TermID=4RequirementID=1</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A88" s="6">
         <v>87</v>
       </c>
@@ -2290,8 +2659,12 @@
       <c r="D88" s="6">
         <v>618</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E88" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=87DegreePlanID=14TermID=4RequirementID=618</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A89" s="6">
         <v>88</v>
       </c>
@@ -2304,8 +2677,12 @@
       <c r="D89" s="6">
         <v>10</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E89" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=88DegreePlanID=14TermID=4RequirementID=10</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A90" s="6">
         <v>89</v>
       </c>
@@ -2318,8 +2695,12 @@
       <c r="D90" s="6">
         <v>691</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E90" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=89DegreePlanID=14TermID=5RequirementID=691</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A91" s="6">
         <v>90</v>
       </c>
@@ -2332,8 +2713,12 @@
       <c r="D91" s="6">
         <v>20</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E91" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=90DegreePlanID=14TermID=5RequirementID=20</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A92" s="6">
         <v>91</v>
       </c>
@@ -2346,8 +2731,12 @@
       <c r="D92" s="6">
         <v>692</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E92" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=91DegreePlanID=14TermID=5RequirementID=692</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A93" s="6">
         <v>92</v>
       </c>
@@ -2360,8 +2749,12 @@
       <c r="D93" s="6">
         <v>460</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E93" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=92DegreePlanID=15TermID=1RequirementID=460</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A94" s="6">
         <v>93</v>
       </c>
@@ -2374,8 +2767,12 @@
       <c r="D94" s="6">
         <v>356</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E94" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=93DegreePlanID=15TermID=1RequirementID=356</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A95" s="6">
         <v>94</v>
       </c>
@@ -2388,8 +2785,12 @@
       <c r="D95" s="6">
         <v>542</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E95" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=94DegreePlanID=15TermID=1RequirementID=542</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A96" s="6">
         <v>95</v>
       </c>
@@ -2402,8 +2803,12 @@
       <c r="D96" s="6">
         <v>563</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E96" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=95DegreePlanID=15TermID=1RequirementID=563</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A97" s="6">
         <v>96</v>
       </c>
@@ -2416,8 +2821,12 @@
       <c r="D97" s="6">
         <v>560</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E97" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=96DegreePlanID=15TermID=2RequirementID=560</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A98" s="6">
         <v>97</v>
       </c>
@@ -2430,8 +2839,12 @@
       <c r="D98" s="6">
         <v>664</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E98" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=97DegreePlanID=15TermID=2RequirementID=664</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A99" s="6">
         <v>98</v>
       </c>
@@ -2444,8 +2857,12 @@
       <c r="D99" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E99" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=98DegreePlanID=15TermID=2RequirementID=1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A100" s="6">
         <v>99</v>
       </c>
@@ -2458,8 +2875,12 @@
       <c r="D100" s="6">
         <v>555</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E100" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=99DegreePlanID=15TermID=3RequirementID=555</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A101" s="6">
         <v>100</v>
       </c>
@@ -2472,8 +2893,12 @@
       <c r="D101" s="6">
         <v>618</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E101" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=100DegreePlanID=15TermID=3RequirementID=618</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A102" s="6">
         <v>101</v>
       </c>
@@ -2486,8 +2911,12 @@
       <c r="D102" s="6">
         <v>691</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E102" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=101DegreePlanID=15TermID=3RequirementID=691</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A103" s="6">
         <v>102</v>
       </c>
@@ -2500,8 +2929,12 @@
       <c r="D103" s="6">
         <v>10</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E103" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=102DegreePlanID=15TermID=4RequirementID=10</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A104" s="6">
         <v>103</v>
       </c>
@@ -2514,8 +2947,12 @@
       <c r="D104" s="6">
         <v>20</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E104" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=103DegreePlanID=15TermID=4RequirementID=20</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A105" s="6">
         <v>104</v>
       </c>
@@ -2527,6 +2964,10 @@
       </c>
       <c r="D105" s="6">
         <v>692</v>
+      </c>
+      <c r="E105" s="9" t="str">
+        <f t="shared" si="1"/>
+        <v>new DegreePlanTermRequirement{DegreePlanTermRequirementID=104DegreePlanID=15TermID=4RequirementID=692</v>
       </c>
     </row>
   </sheetData>
@@ -2536,10 +2977,10 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2711,7 +3152,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2809,7 +3250,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>